<commit_message>
payments plan to product folder
</commit_message>
<xml_diff>
--- a/Data Files/Payments/Payments module.xlsx
+++ b/Data Files/Payments/Payments module.xlsx
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="paymentplannames" sheetId="2" r:id="rId2"/>
+    <sheet name="paymentplan" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Approval status</t>
   </si>
@@ -51,49 +51,43 @@
     <t>Display Name (Marketing):</t>
   </si>
   <si>
-    <t>M-kopa test 10</t>
-  </si>
-  <si>
-    <t>M-kopa test 11</t>
-  </si>
-  <si>
-    <t>M-kopa test 12</t>
-  </si>
-  <si>
-    <t>M-kopa test 13</t>
-  </si>
-  <si>
-    <t>M-kopa test 14</t>
-  </si>
-  <si>
-    <t>M-kopa test 15</t>
-  </si>
-  <si>
-    <t>M-kopa test 16</t>
-  </si>
-  <si>
-    <t>M-kopa test 17</t>
-  </si>
-  <si>
-    <t>M-kopa test 18</t>
-  </si>
-  <si>
-    <t>M-kopa test 19</t>
-  </si>
-  <si>
-    <t>M-kopa test 20</t>
-  </si>
-  <si>
-    <t>M-kopa test 21</t>
-  </si>
-  <si>
-    <t>M-kopa test 22</t>
-  </si>
-  <si>
-    <t>M-kopa test 23</t>
-  </si>
-  <si>
-    <t>M-kopa test 24</t>
+    <t>cashprice</t>
+  </si>
+  <si>
+    <t>loanDepoit</t>
+  </si>
+  <si>
+    <t>Freeusage</t>
+  </si>
+  <si>
+    <t>costpercredit</t>
+  </si>
+  <si>
+    <t>days</t>
+  </si>
+  <si>
+    <t>loantotalprice</t>
+  </si>
+  <si>
+    <t>Approvernotes</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>M-kopa test 26</t>
+  </si>
+  <si>
+    <t>M-kopa test 27</t>
+  </si>
+  <si>
+    <t>M-kopa test 28</t>
+  </si>
+  <si>
+    <t>M-kopa test 29</t>
+  </si>
+  <si>
+    <t>M-kopa test 30</t>
   </si>
 </sst>
 </file>
@@ -468,10 +462,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B10"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -480,132 +474,94 @@
     <col min="2" max="2" width="22.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="C2">
+        <v>63000</v>
+      </c>
+      <c r="D2">
+        <v>2999</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>55</v>
+      </c>
+      <c r="G2">
+        <v>365</v>
+      </c>
+      <c r="H2">
+        <v>65000</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>